<commit_message>
Added some documentary comments, included identification rules and fixed one rule that was wrong (project membership)
</commit_message>
<xml_diff>
--- a/Examples/ProjectAdministration/ProjectAdministration.xlsx
+++ b/Examples/ProjectAdministration/ProjectAdministration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="18195" windowHeight="11760"/>
+    <workbookView xWindow="480" yWindow="96" windowWidth="18192" windowHeight="11016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="82">
   <si>
     <t>Project</t>
   </si>
@@ -169,9 +169,6 @@
     <t>P. Leider</t>
   </si>
   <si>
-    <t>Niet meer in dienst.</t>
-  </si>
-  <si>
     <t>pleider@example.com</t>
   </si>
   <si>
@@ -254,6 +251,15 @@
   </si>
   <si>
     <t>completed</t>
+  </si>
+  <si>
+    <t>has left the company</t>
+  </si>
+  <si>
+    <t>maternity leave</t>
+  </si>
+  <si>
+    <t>is on sabbatical until 4th of July</t>
   </si>
 </sst>
 </file>
@@ -624,22 +630,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="58.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1"/>
+    <col min="4" max="4" width="58.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" style="8" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="33.42578125" customWidth="1"/>
+    <col min="7" max="7" width="33.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -662,21 +668,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="D2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>0</v>
@@ -685,7 +691,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -693,10 +699,10 @@
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E3" s="8">
         <v>41639</v>
@@ -708,7 +714,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -716,10 +722,10 @@
         <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" s="8">
         <v>41685</v>
@@ -731,7 +737,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>22</v>
       </c>
@@ -739,7 +745,7 @@
         <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E5" s="8">
         <v>41835</v>
@@ -748,7 +754,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -756,14 +762,14 @@
         <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E6" s="8"/>
       <c r="G6" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>26</v>
       </c>
@@ -771,7 +777,7 @@
         <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="5" t="s">
@@ -781,7 +787,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>29</v>
       </c>
@@ -789,10 +795,10 @@
         <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E8" s="8">
         <v>25675</v>
@@ -804,12 +810,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="3"/>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
@@ -818,7 +824,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>0</v>
       </c>
@@ -827,7 +833,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>8</v>
       </c>
@@ -835,7 +841,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>8</v>
       </c>
@@ -843,7 +849,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>8</v>
       </c>
@@ -851,7 +857,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>18</v>
       </c>
@@ -859,7 +865,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -867,7 +873,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>18</v>
       </c>
@@ -875,7 +881,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>18</v>
       </c>
@@ -883,7 +889,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>22</v>
       </c>
@@ -891,7 +897,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
@@ -899,7 +905,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>22</v>
       </c>
@@ -907,7 +913,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>29</v>
       </c>
@@ -915,7 +921,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>29</v>
       </c>
@@ -923,7 +929,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>29</v>
       </c>
@@ -931,7 +937,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>35</v>
       </c>
@@ -946,22 +952,22 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>15</v>
       </c>
@@ -969,13 +975,13 @@
         <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>16</v>
       </c>
@@ -983,35 +989,38 @@
         <v>40</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B30" t="s">
         <v>41</v>
       </c>
+      <c r="C30" t="s">
+        <v>80</v>
+      </c>
       <c r="D30" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B31" t="s">
         <v>42</v>
       </c>
-      <c r="C31" t="s">
-        <v>51</v>
+      <c r="C31" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>21</v>
       </c>
@@ -1019,10 +1028,10 @@
         <v>43</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>33</v>
       </c>
@@ -1030,10 +1039,10 @@
         <v>44</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>28</v>
       </c>
@@ -1041,10 +1050,10 @@
         <v>45</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>31</v>
       </c>
@@ -1052,10 +1061,10 @@
         <v>46</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>32</v>
       </c>
@@ -1063,10 +1072,10 @@
         <v>47</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>34</v>
       </c>
@@ -1074,21 +1083,24 @@
         <v>48</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B38" t="s">
         <v>49</v>
       </c>
+      <c r="C38" t="s">
+        <v>81</v>
+      </c>
       <c r="D38" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>14</v>
       </c>
@@ -1096,7 +1108,7 @@
         <v>50</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>